<commit_message>
Update pits excel as well
</commit_message>
<xml_diff>
--- a/2022_app/2022_app/2022_scouting_app/leaderscripts/ScoutingData_template.xlsx
+++ b/2022_app/2022_app/2022_scouting_app/leaderscripts/ScoutingData_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brrice-my.sharepoint.com/personal/23kongw_brrice_edu/Documents/Documents/GitHub/2022_Scouting_App_FRC_573/2022_app/2022_app/2022_scouting_app/leaderscripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_F360F36165E143200E71C5BFB84F5EBB8D8ED7C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A524A18-83C6-44F7-AE32-E61CEF7EAA06}"/>
+  <xr:revisionPtr revIDLastSave="58" documentId="11_F360F36165E143200E71C5BFB84F5EBB8D8ED7C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A833239-8C60-42E5-8210-943DC7A1784E}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -518,6 +518,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -526,12 +534,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -542,8 +544,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -890,21 +890,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
       <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:45" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="A2" s="27"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
       <c r="F2" s="13"/>
     </row>
     <row r="4" spans="1:45" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -978,60 +978,60 @@
       <c r="B7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="25" t="s">
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="25" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="30"/>
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="30"/>
+      <c r="O7" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="25" t="s">
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="26"/>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="26"/>
-      <c r="AA7" s="25" t="s">
+      <c r="T7" s="30"/>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="30"/>
+      <c r="X7" s="30"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="AB7" s="26"/>
-      <c r="AC7" s="26"/>
-      <c r="AD7" s="27"/>
-      <c r="AE7" s="25" t="s">
+      <c r="AB7" s="30"/>
+      <c r="AC7" s="30"/>
+      <c r="AD7" s="31"/>
+      <c r="AE7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="AF7" s="26"/>
-      <c r="AG7" s="26"/>
-      <c r="AH7" s="26"/>
-      <c r="AI7" s="26"/>
-      <c r="AJ7" s="26"/>
-      <c r="AK7" s="26"/>
-      <c r="AL7" s="26"/>
-      <c r="AM7" s="25"/>
-      <c r="AN7" s="26"/>
-      <c r="AO7" s="26"/>
-      <c r="AP7" s="26"/>
-      <c r="AQ7" s="26"/>
-      <c r="AR7" s="27"/>
+      <c r="AF7" s="30"/>
+      <c r="AG7" s="30"/>
+      <c r="AH7" s="30"/>
+      <c r="AI7" s="30"/>
+      <c r="AJ7" s="30"/>
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="30"/>
+      <c r="AM7" s="29"/>
+      <c r="AN7" s="30"/>
+      <c r="AO7" s="30"/>
+      <c r="AP7" s="30"/>
+      <c r="AQ7" s="30"/>
+      <c r="AR7" s="31"/>
     </row>
     <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
@@ -1214,6 +1214,8 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="AM6:AR6"/>
+    <mergeCell ref="AM7:AR7"/>
     <mergeCell ref="A1:E2"/>
     <mergeCell ref="O6:Z6"/>
     <mergeCell ref="AA6:AL6"/>
@@ -1223,8 +1225,6 @@
     <mergeCell ref="S7:Z7"/>
     <mergeCell ref="AA7:AD7"/>
     <mergeCell ref="AE7:AL7"/>
-    <mergeCell ref="AM6:AR6"/>
-    <mergeCell ref="AM7:AR7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1621,7 +1621,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1663,10 +1663,10 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="32"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -1729,20 +1729,20 @@
       <c r="D16" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="26" t="s">
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="33"/>
-      <c r="M16" s="33"/>
-      <c r="N16" s="34"/>
+      <c r="J16" s="30"/>
+      <c r="K16" s="30"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="26"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">

</xml_diff>

<commit_message>
Update excel script and Add ending location to the summary page
</commit_message>
<xml_diff>
--- a/2022_app/2022_app/2022_scouting_app/leaderscripts/ScoutingData_template.xlsx
+++ b/2022_app/2022_app/2022_scouting_app/leaderscripts/ScoutingData_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brrice-my.sharepoint.com/personal/23kongw_brrice_edu/Documents/Documents/GitHub/2022_Scouting_App_FRC_573/2022_app/2022_app/2022_scouting_app/leaderscripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="11_F360F36165E143200E71C5BFB84F5EBB8D8ED7C2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A833239-8C60-42E5-8210-943DC7A1784E}"/>
+  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{C87C93F0-9EB4-44FE-BCD5-360F9FBCBFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99CD4814-4E04-42CA-9719-94AD05879231}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <sheet name="template" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$8:$AJ$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$8:$Z$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>Team Number</t>
   </si>
@@ -142,42 +142,15 @@
     <t>Not Us</t>
   </si>
   <si>
-    <t>Climb time (in sec)</t>
-  </si>
-  <si>
     <t>Upper</t>
   </si>
   <si>
-    <t>Inner</t>
-  </si>
-  <si>
     <t>Lower</t>
   </si>
   <si>
-    <t>Crossline</t>
-  </si>
-  <si>
-    <t>Position Control</t>
-  </si>
-  <si>
-    <t>Level Climb</t>
-  </si>
-  <si>
-    <t>Buddy Climb</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
-    <t>Color Wheel Adjustment</t>
-  </si>
-  <si>
-    <t>Color Wheel Sensors</t>
-  </si>
-  <si>
-    <t>Open to using our Buddy Climb</t>
-  </si>
-  <si>
     <t>Strengths</t>
   </si>
   <si>
@@ -265,12 +238,6 @@
     <t>The School at Marygrove</t>
   </si>
   <si>
-    <t>Rotational Control</t>
-  </si>
-  <si>
-    <t>Cimb</t>
-  </si>
-  <si>
     <t>Auto</t>
   </si>
   <si>
@@ -293,6 +260,12 @@
   </si>
   <si>
     <t>Ending Location</t>
+  </si>
+  <si>
+    <t>Upper2</t>
+  </si>
+  <si>
+    <t>Lower3</t>
   </si>
 </sst>
 </file>
@@ -371,7 +344,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -464,11 +437,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -503,28 +572,58 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -535,8 +634,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -548,7 +653,295 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -559,6 +952,37 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F89A9134-5A48-4690-8E03-B41419A45991}" name="Table5" displayName="Table5" ref="A16:L20" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
+  <autoFilter ref="A16:L20" xr:uid="{F89A9134-5A48-4690-8E03-B41419A45991}"/>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{F16D52E8-F1B0-4725-9A27-45D91C19A5A4}" name="Match #" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{3726BEAE-513B-47AE-A1AE-66F34444D173}" name="Alliance Color" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{C971C71B-CEBE-461E-B3C0-B5468140EF01}" name="Scouter Name" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{FEEE8CF9-038E-47FE-9A89-C746D53691F2}" name="Starting Location"/>
+    <tableColumn id="5" xr3:uid="{73624BFB-8EC0-4B5C-89EA-8A36B95A15D7}" name="Upper" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{C2F0C0CE-ABBF-494D-8360-E886D43B1D5B}" name="Lower" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{0DFDE256-C59F-45F3-A998-E024897F9A27}" name="Leave TARMAC" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{738F6C5C-DEE0-4635-8D26-EC6F98C7864D}" name="Human Player Score" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{42EB9B00-AE97-4FC3-BBBD-481E41257273}" name="Upper2" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{D01BB072-7A5B-4A74-89D7-756AD36CF372}" name="Lower3" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{CAD660AF-D41C-448C-ABE2-C6A38E71B326}" name="Ending Location" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{6A6E1A69-8D5E-4BC3-97EB-6D439DAC7BAD}" name="Notes" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{351508BC-A90F-4BCF-A6C7-5EE7B6956DF7}" name="Table7" displayName="Table7" ref="A1:A12" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:A12" xr:uid="{351508BC-A90F-4BCF-A6C7-5EE7B6956DF7}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{EC75A18F-7806-48C6-B018-3520F72D5CF8}" name="Team Number"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -846,74 +1270,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AS11"/>
+  <dimension ref="A1:AP11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.54296875" customWidth="1"/>
-    <col min="18" max="20" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="24" max="26" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.7265625" customWidth="1"/>
-    <col min="29" max="29" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="32" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="33" max="35" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8.81640625" customWidth="1"/>
+    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="26" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
       <c r="F1" s="13"/>
     </row>
-    <row r="2" spans="1:45" ht="26" x14ac:dyDescent="0.35">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
+    <row r="2" spans="1:42" ht="26" x14ac:dyDescent="0.35">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="4" spans="1:45" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" ht="23.5" x14ac:dyDescent="0.35">
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:45" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" ht="23.5" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -921,256 +1349,193 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:45" ht="23.5" x14ac:dyDescent="0.35">
-      <c r="B6" s="23" t="s">
+    <row r="6" spans="1:42" ht="23.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="22"/>
+      <c r="B6" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24"/>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24"/>
-      <c r="N6" s="24"/>
-      <c r="O6" s="28" t="s">
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="P6" s="28"/>
-      <c r="Q6" s="28"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="28"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
-      <c r="X6" s="28"/>
-      <c r="Y6" s="28"/>
-      <c r="Z6" s="28"/>
-      <c r="AA6" s="28" t="s">
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="AB6" s="28"/>
-      <c r="AC6" s="28"/>
-      <c r="AD6" s="28"/>
-      <c r="AE6" s="28"/>
-      <c r="AF6" s="28"/>
-      <c r="AG6" s="28"/>
-      <c r="AH6" s="28"/>
-      <c r="AI6" s="28"/>
-      <c r="AJ6" s="28"/>
-      <c r="AK6" s="28"/>
-      <c r="AL6" s="28"/>
-      <c r="AM6" s="28" t="s">
+      <c r="R6" s="40"/>
+      <c r="S6" s="40"/>
+      <c r="T6" s="40"/>
+      <c r="U6" s="40"/>
+      <c r="V6" s="40"/>
+      <c r="W6" s="40"/>
+      <c r="X6" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="AN6" s="28"/>
-      <c r="AO6" s="28"/>
-      <c r="AP6" s="28"/>
-      <c r="AQ6" s="28"/>
-      <c r="AR6" s="28"/>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="Y6" s="40"/>
+      <c r="Z6" s="40"/>
+      <c r="AA6" s="21"/>
+      <c r="AB6" s="21"/>
+      <c r="AC6" s="21"/>
+      <c r="AD6" s="21"/>
+      <c r="AE6" s="21"/>
+      <c r="AF6" s="21"/>
+      <c r="AG6" s="21"/>
+      <c r="AH6" s="21"/>
+      <c r="AI6" s="21"/>
+      <c r="AJ6" s="21"/>
+      <c r="AK6" s="21"/>
+      <c r="AL6" s="21"/>
+      <c r="AM6" s="21"/>
+      <c r="AN6" s="21"/>
+      <c r="AO6" s="21"/>
+      <c r="AP6" s="21"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A7" s="22"/>
       <c r="B7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="30"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="29" t="s">
+      <c r="C7" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="30"/>
-      <c r="I7" s="30"/>
-      <c r="J7" s="30"/>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="30"/>
-      <c r="N7" s="30"/>
-      <c r="O7" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="31"/>
-      <c r="S7" s="29" t="s">
+      <c r="H7" s="44"/>
+      <c r="I7" s="45"/>
+      <c r="J7" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
+      <c r="M7" s="42"/>
+      <c r="N7" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="T7" s="30"/>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="30"/>
-      <c r="X7" s="30"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB7" s="30"/>
-      <c r="AC7" s="30"/>
-      <c r="AD7" s="31"/>
-      <c r="AE7" s="29" t="s">
+      <c r="O7" s="44"/>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="R7" s="42"/>
+      <c r="S7" s="42"/>
+      <c r="T7" s="42"/>
+      <c r="U7" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="AF7" s="30"/>
-      <c r="AG7" s="30"/>
-      <c r="AH7" s="30"/>
-      <c r="AI7" s="30"/>
-      <c r="AJ7" s="30"/>
-      <c r="AK7" s="30"/>
-      <c r="AL7" s="30"/>
-      <c r="AM7" s="29"/>
-      <c r="AN7" s="30"/>
-      <c r="AO7" s="30"/>
-      <c r="AP7" s="30"/>
-      <c r="AQ7" s="30"/>
-      <c r="AR7" s="31"/>
-    </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
-      <c r="A8" s="4" t="s">
+      <c r="V7" s="42"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="40"/>
+      <c r="Y7" s="40"/>
+      <c r="Z7" s="40"/>
+      <c r="AA7" s="11"/>
+      <c r="AB7" s="11"/>
+      <c r="AC7" s="11"/>
+      <c r="AD7" s="11"/>
+      <c r="AE7" s="11"/>
+      <c r="AF7" s="11"/>
+      <c r="AG7" s="11"/>
+      <c r="AH7" s="11"/>
+      <c r="AI7" s="11"/>
+      <c r="AJ7" s="11"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="11"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+      <c r="A8" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>35</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="Q8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="S8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="T8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="X8" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y8" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="T8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="V8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="X8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AI8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ8" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AL8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM8" t="s">
-        <v>47</v>
-      </c>
-      <c r="AN8" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AP8" t="s">
-        <v>45</v>
-      </c>
-      <c r="AQ8" t="s">
-        <v>34</v>
-      </c>
-      <c r="AR8" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS8" t="s">
+      <c r="Z8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -1185,13 +1550,11 @@
       <c r="L10" s="11"/>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
+      <c r="O10" s="10"/>
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
-      <c r="R10" s="10"/>
-      <c r="S10" s="10"/>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="12"/>
@@ -1209,22 +1572,20 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
       <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AM6:AR6"/>
-    <mergeCell ref="AM7:AR7"/>
+    <mergeCell ref="Q6:W6"/>
+    <mergeCell ref="X6:Z7"/>
     <mergeCell ref="A1:E2"/>
-    <mergeCell ref="O6:Z6"/>
-    <mergeCell ref="AA6:AL6"/>
     <mergeCell ref="C7:F7"/>
-    <mergeCell ref="G7:N7"/>
-    <mergeCell ref="O7:R7"/>
-    <mergeCell ref="S7:Z7"/>
-    <mergeCell ref="AA7:AD7"/>
-    <mergeCell ref="AE7:AL7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="U7:W7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J6:P6"/>
+    <mergeCell ref="N7:P7"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -1252,8 +1613,8 @@
       <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="22"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="F2">
@@ -1276,7 +1637,7 @@
         <v>240</v>
       </c>
       <c r="G4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
@@ -1284,7 +1645,7 @@
         <v>247</v>
       </c>
       <c r="G5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -1292,7 +1653,7 @@
         <v>548</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -1324,7 +1685,7 @@
         <v>2591</v>
       </c>
       <c r="G10" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
@@ -1332,7 +1693,7 @@
         <v>3096</v>
       </c>
       <c r="G11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -1340,7 +1701,7 @@
         <v>3414</v>
       </c>
       <c r="G12" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
@@ -1356,7 +1717,7 @@
         <v>4130</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
@@ -1372,7 +1733,7 @@
         <v>4768</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="6:7" x14ac:dyDescent="0.35">
@@ -1396,7 +1757,7 @@
         <v>5090</v>
       </c>
       <c r="G19" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="6:7" x14ac:dyDescent="0.35">
@@ -1412,7 +1773,7 @@
         <v>5214</v>
       </c>
       <c r="G21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="6:7" x14ac:dyDescent="0.35">
@@ -1420,7 +1781,7 @@
         <v>5498</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="6:7" x14ac:dyDescent="0.35">
@@ -1436,7 +1797,7 @@
         <v>5532</v>
       </c>
       <c r="G24" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="6:7" x14ac:dyDescent="0.35">
@@ -1444,7 +1805,7 @@
         <v>5577</v>
       </c>
       <c r="G25" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="6:7" x14ac:dyDescent="0.35">
@@ -1452,7 +1813,7 @@
         <v>5695</v>
       </c>
       <c r="G26" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.35">
@@ -1460,7 +1821,7 @@
         <v>5756</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="6:7" x14ac:dyDescent="0.35">
@@ -1468,7 +1829,7 @@
         <v>6013</v>
       </c>
       <c r="G28" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
     </row>
     <row r="29" spans="6:7" x14ac:dyDescent="0.35">
@@ -1476,7 +1837,7 @@
         <v>6120</v>
       </c>
       <c r="G29" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="6:7" x14ac:dyDescent="0.35">
@@ -1484,7 +1845,7 @@
         <v>6742</v>
       </c>
       <c r="G30" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
     </row>
     <row r="31" spans="6:7" x14ac:dyDescent="0.35">
@@ -1492,7 +1853,7 @@
         <v>7145</v>
       </c>
       <c r="G31" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="6:7" x14ac:dyDescent="0.35">
@@ -1500,7 +1861,7 @@
         <v>7191</v>
       </c>
       <c r="G32" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="6:7" x14ac:dyDescent="0.35">
@@ -1524,7 +1885,7 @@
         <v>7692</v>
       </c>
       <c r="G35" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.35">
@@ -1532,7 +1893,7 @@
         <v>7716</v>
       </c>
       <c r="G36" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.35">
@@ -1540,7 +1901,7 @@
         <v>7783</v>
       </c>
       <c r="G37" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.35">
@@ -1548,7 +1909,7 @@
         <v>7856</v>
       </c>
       <c r="G38" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="6:7" x14ac:dyDescent="0.35">
@@ -1556,7 +1917,7 @@
         <v>7865</v>
       </c>
       <c r="G39" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="6:7" x14ac:dyDescent="0.35">
@@ -1564,7 +1925,7 @@
         <v>8179</v>
       </c>
       <c r="G40" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
     </row>
     <row r="41" spans="6:7" x14ac:dyDescent="0.35">
@@ -1572,7 +1933,7 @@
         <v>8280</v>
       </c>
       <c r="G41" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -1618,23 +1979,25 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.453125" customWidth="1"/>
     <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="16.26953125" customWidth="1"/>
     <col min="5" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7265625" customWidth="1"/>
-    <col min="8" max="8" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.54296875" customWidth="1"/>
+    <col min="8" max="8" width="18.6328125" customWidth="1"/>
+    <col min="9" max="9" width="8.6328125" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.36328125" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.1796875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.6328125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="7.90625" bestFit="1" customWidth="1"/>
@@ -1648,7 +2011,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="16"/>
@@ -1663,50 +2026,50 @@
       <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="32"/>
+      <c r="B4" s="30"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B10" s="17"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B11" s="17"/>
     </row>
@@ -1716,230 +2079,234 @@
       </c>
       <c r="B12" s="17"/>
     </row>
-    <row r="13" spans="1:14" ht="112" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>9</v>
-      </c>
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="50"/>
+      <c r="I15" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="26"/>
+      <c r="N15" s="27"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="J16" s="30"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="26"/>
+      <c r="A16" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="36" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="H16" s="36" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="L16" s="37" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="A17" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="4" t="e">
+        <f>AVERAGE(E21:E220)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F17" s="4" t="e">
+        <f t="shared" ref="F17:K17" si="0">AVERAGE(F21:F220)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G17" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H17" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I17" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J17" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="K17" s="4" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L17" s="33"/>
+      <c r="M17" s="18"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A18" s="4" t="s">
-        <v>42</v>
+      <c r="A18" s="31" t="s">
+        <v>7</v>
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="6"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="4" t="e">
-        <f>AVERAGE(E21:E45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F18" s="4" t="e">
-        <f t="shared" ref="F18:G18" si="0">AVERAGE(F21:F45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G18" s="4" t="e">
-        <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="H18" s="4" t="e">
-        <f>AVERAGE(I21:I45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I18" s="4" t="e">
-        <f>AVERAGE(J21:J45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J18" s="4" t="e">
-        <f>AVERAGE(K21:K45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K18" s="4" t="e">
-        <f>AVERAGE(L22:L45)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="L18" s="18"/>
-      <c r="M18" s="19"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A19" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="4">
-        <f>MAX(E21:E45)</f>
+      <c r="D18" s="6"/>
+      <c r="E18" s="4">
+        <f>MAX(E21:E200)</f>
         <v>0</v>
       </c>
-      <c r="F19" s="4">
-        <f>MAX(H21:H45)</f>
+      <c r="F18" s="4">
+        <f t="shared" ref="F18:K18" si="1">MAX(F21:F200)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G18" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19" s="4">
-        <f>MAX(I21:I45)</f>
+      <c r="H18" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I19" s="4">
-        <f>MAX(J21:J45)</f>
+      <c r="I18" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J19" s="4">
-        <f>MAX(K21:K45)</f>
+      <c r="J18" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K19" s="4">
-        <f>MAX(L22:L45)</f>
+      <c r="K18" s="4">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L19" s="18"/>
-      <c r="M19" s="19"/>
-    </row>
-    <row r="20" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="5" t="s">
+      <c r="L18" s="33"/>
+      <c r="M18" s="18"/>
+    </row>
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="5">
-        <f>MIN(E21:E45)</f>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="5">
+        <f>MIN(E21:E200)</f>
         <v>0</v>
       </c>
-      <c r="F20" s="5">
-        <f>MIN(H21:H45)</f>
+      <c r="F19" s="5">
+        <f t="shared" ref="F19:K19" si="2">MIN(F21:F200)</f>
         <v>0</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G19" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="H20" s="5">
-        <f>MIN(I21:I45)</f>
+      <c r="H19" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I20" s="5">
-        <f>MIN(J21:J45)</f>
+      <c r="I19" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J20" s="5">
-        <f>MIN(K21:K45)</f>
+      <c r="J19" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K20" s="5">
-        <f>MIN(L22:L45)</f>
+      <c r="K19" s="5">
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L20" s="20"/>
-      <c r="M20" s="19"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="L19" s="34"/>
+      <c r="M19" s="18"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B20" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C20" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="2" t="s">
+      <c r="D20" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="G20" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="J21" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="K21" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="L21" s="2" t="s">
+      <c r="K20" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="L20" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="M21" s="19"/>
+      <c r="M20" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="E16:H16"/>
-    <mergeCell ref="I16:K16"/>
+  <mergeCells count="2">
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="I15:L15"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update with Milford team list
</commit_message>
<xml_diff>
--- a/2022_app/2022_app/2022_scouting_app/leaderscripts/ScoutingData_template.xlsx
+++ b/2022_app/2022_app/2022_scouting_app/leaderscripts/ScoutingData_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://brrice-my.sharepoint.com/personal/23kongw_brrice_edu/Documents/Documents/GitHub/2022_Scouting_App_FRC_573/2022_app/2022_app/2022_scouting_app/leaderscripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\savag\Documents\GitHub\2022_Scouting_App_FRC_573\2022_app\2022_app\2022_scouting_app\leaderscripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="13_ncr:1_{C87C93F0-9EB4-44FE-BCD5-360F9FBCBFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99CD4814-4E04-42CA-9719-94AD05879231}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598E1E98-1449-42C4-AED1-657182B5FE5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="109">
   <si>
     <t>Team Number</t>
   </si>
@@ -139,9 +139,6 @@
     <t>Level</t>
   </si>
   <si>
-    <t>Not Us</t>
-  </si>
-  <si>
     <t>Upper</t>
   </si>
   <si>
@@ -266,13 +263,115 @@
   </si>
   <si>
     <t>Lower3</t>
+  </si>
+  <si>
+    <t>The HOT Team</t>
+  </si>
+  <si>
+    <t>Monsters</t>
+  </si>
+  <si>
+    <t>Rockem Sockem Robotics</t>
+  </si>
+  <si>
+    <t>Frog Force</t>
+  </si>
+  <si>
+    <t>The RatPack</t>
+  </si>
+  <si>
+    <t>Lightning Robotics</t>
+  </si>
+  <si>
+    <t>Technical Difficulties</t>
+  </si>
+  <si>
+    <t>The Fighting Pi</t>
+  </si>
+  <si>
+    <t>HAZMATs</t>
+  </si>
+  <si>
+    <t>The Charge</t>
+  </si>
+  <si>
+    <t>Bionic Black Hawks</t>
+  </si>
+  <si>
+    <t>Waterford Robotics</t>
+  </si>
+  <si>
+    <t>Brighton TechnoDogs</t>
+  </si>
+  <si>
+    <t>CSPA Gems</t>
+  </si>
+  <si>
+    <t>The Atoms Family</t>
+  </si>
+  <si>
+    <t>Robo-Bucs</t>
+  </si>
+  <si>
+    <t>Raider Robotics</t>
+  </si>
+  <si>
+    <t>Hemlock's Gray Matter</t>
+  </si>
+  <si>
+    <t>CC Shambots</t>
+  </si>
+  <si>
+    <t>Whiteford Bobcats</t>
+  </si>
+  <si>
+    <t>Yeti</t>
+  </si>
+  <si>
+    <t>Hollywood</t>
+  </si>
+  <si>
+    <t>Mechatronic Mustangs</t>
+  </si>
+  <si>
+    <t>Knowmads</t>
+  </si>
+  <si>
+    <t>OSTC - SWEET BOTS</t>
+  </si>
+  <si>
+    <t>SCA Constellations</t>
+  </si>
+  <si>
+    <t>The Byting Irish</t>
+  </si>
+  <si>
+    <t>Lincoln Abes</t>
+  </si>
+  <si>
+    <t>Robo Falcons</t>
+  </si>
+  <si>
+    <t>Techno Falcons</t>
+  </si>
+  <si>
+    <t>Toro Loco</t>
+  </si>
+  <si>
+    <t>Cyber Tigers West</t>
+  </si>
+  <si>
+    <t>Automated Amphibians</t>
+  </si>
+  <si>
+    <t>Bubo's Parliament</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +408,13 @@
       <sz val="7"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Segoe UI"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -537,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -648,6 +754,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1276,48 +1385,48 @@
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="6" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.90625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.6328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="28" max="30" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="31" max="33" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="34" max="36" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8.81640625" customWidth="1"/>
+    <col min="24" max="24" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="30" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="33" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="26" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A1" s="41" t="s">
         <v>23</v>
       </c>
@@ -1327,7 +1436,7 @@
       <c r="E1" s="41"/>
       <c r="F1" s="13"/>
     </row>
-    <row r="2" spans="1:42" ht="26" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A2" s="41"/>
       <c r="B2" s="41"/>
       <c r="C2" s="41"/>
@@ -1335,13 +1444,13 @@
       <c r="E2" s="41"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="4" spans="1:42" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
       <c r="E4" s="9"/>
       <c r="F4" s="9"/>
     </row>
-    <row r="5" spans="1:42" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -1349,7 +1458,7 @@
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
     </row>
-    <row r="6" spans="1:42" ht="23.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:42" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="40" t="s">
         <v>24</v>
@@ -1401,13 +1510,13 @@
       <c r="AO6" s="21"/>
       <c r="AP6" s="21"/>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="15" t="s">
         <v>30</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D7" s="42"/>
       <c r="E7" s="42"/>
@@ -1418,7 +1527,7 @@
       <c r="H7" s="44"/>
       <c r="I7" s="45"/>
       <c r="J7" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
@@ -1429,7 +1538,7 @@
       <c r="O7" s="44"/>
       <c r="P7" s="45"/>
       <c r="Q7" s="42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42"/>
@@ -1455,7 +1564,7 @@
       <c r="AK7" s="11"/>
       <c r="AL7" s="11"/>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>0</v>
       </c>
@@ -1463,79 +1572,79 @@
         <v>32</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="G8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="I8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="J8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="K8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="L8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M8" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="N8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="P8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="R8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="S8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="T8" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T8" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="U8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="V8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="V8" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="W8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="X8" s="24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Z8" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
       <c r="C10" s="11"/>
@@ -1554,7 +1663,7 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
       <c r="C11" s="12"/>
@@ -1600,13 +1709,13 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>573</v>
       </c>
@@ -1616,7 +1725,7 @@
       <c r="F1" s="19"/>
       <c r="G1" s="20"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F2">
         <v>33</v>
       </c>
@@ -1624,7 +1733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F3">
         <v>94</v>
       </c>
@@ -1632,31 +1741,31 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F4">
         <v>240</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F5">
         <v>247</v>
       </c>
       <c r="G5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F6">
         <v>548</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F7">
         <v>573</v>
       </c>
@@ -1664,7 +1773,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F8">
         <v>835</v>
       </c>
@@ -1672,7 +1781,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F9">
         <v>1481</v>
       </c>
@@ -1680,31 +1789,31 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F10">
         <v>2591</v>
       </c>
       <c r="G10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F11">
         <v>3096</v>
       </c>
       <c r="G11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F12">
         <v>3414</v>
       </c>
       <c r="G12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F13">
         <v>3538</v>
       </c>
@@ -1712,15 +1821,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F14">
         <v>4130</v>
       </c>
       <c r="G14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F15">
         <v>4758</v>
       </c>
@@ -1728,15 +1837,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F16">
         <v>4768</v>
       </c>
       <c r="G16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="6:7" x14ac:dyDescent="0.35">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F17">
         <v>4840</v>
       </c>
@@ -1744,7 +1853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F18">
         <v>4854</v>
       </c>
@@ -1752,15 +1861,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F19">
         <v>5090</v>
       </c>
       <c r="G19" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="20" spans="6:7" x14ac:dyDescent="0.35">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F20">
         <v>5197</v>
       </c>
@@ -1768,23 +1877,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F21">
         <v>5214</v>
       </c>
       <c r="G21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="6:7" x14ac:dyDescent="0.35">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F22">
         <v>5498</v>
       </c>
       <c r="G22" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="23" spans="6:7" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F23">
         <v>5531</v>
       </c>
@@ -1792,79 +1901,79 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24">
         <v>5532</v>
       </c>
       <c r="G24" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.35">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F25">
         <v>5577</v>
       </c>
       <c r="G25" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="6:7" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F26">
         <v>5695</v>
       </c>
       <c r="G26" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.35">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F27">
         <v>5756</v>
       </c>
       <c r="G27" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="28" spans="6:7" x14ac:dyDescent="0.35">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F28">
         <v>6013</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="6:7" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F29">
         <v>6120</v>
       </c>
       <c r="G29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="6:7" x14ac:dyDescent="0.35">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F30">
         <v>6742</v>
       </c>
       <c r="G30" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="31" spans="6:7" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F31">
         <v>7145</v>
       </c>
       <c r="G31" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="32" spans="6:7" x14ac:dyDescent="0.35">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F32">
         <v>7191</v>
       </c>
       <c r="G32" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.35">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F33">
         <v>7218</v>
       </c>
@@ -1872,7 +1981,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F34">
         <v>7232</v>
       </c>
@@ -1880,60 +1989,60 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F35">
         <v>7692</v>
       </c>
       <c r="G35" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.35">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36">
         <v>7716</v>
       </c>
       <c r="G36" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37">
         <v>7783</v>
       </c>
       <c r="G37" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.35">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F38">
         <v>7856</v>
       </c>
       <c r="G38" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="6:7" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F39">
         <v>7865</v>
       </c>
       <c r="G39" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F40">
         <v>8179</v>
       </c>
       <c r="G40" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="6:7" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F41">
         <v>8280</v>
       </c>
       <c r="G41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1944,31 +2053,320 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A1">
+        <v>67</v>
+      </c>
+      <c r="B1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>240</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>308</v>
+      </c>
+      <c r="B3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>453</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>503</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>573</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>830</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>862</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1481</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>1502</v>
+      </c>
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1718</v>
+      </c>
+      <c r="B11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2145</v>
+      </c>
+      <c r="B12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2619</v>
+      </c>
+      <c r="B13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2834</v>
+      </c>
+      <c r="B14" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3098</v>
+      </c>
+      <c r="B15" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3707</v>
+      </c>
+      <c r="B16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4362</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>4405</v>
+      </c>
+      <c r="B18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>5263</v>
+      </c>
+      <c r="B19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>5561</v>
+      </c>
+      <c r="B20" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5712</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>5907</v>
+      </c>
+      <c r="B22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>6570</v>
+      </c>
+      <c r="B23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>7178</v>
+      </c>
+      <c r="B24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>7211</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>7225</v>
+      </c>
+      <c r="B26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>7254</v>
+      </c>
+      <c r="B27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>7553</v>
+      </c>
+      <c r="B28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>7598</v>
+      </c>
+      <c r="B29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>7660</v>
+      </c>
+      <c r="B30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>7791</v>
+      </c>
+      <c r="B31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>8179</v>
+      </c>
+      <c r="B32" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8299</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>8361</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>8362</v>
+      </c>
+      <c r="B35" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>8426</v>
+      </c>
+      <c r="B36" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>8519</v>
+      </c>
+      <c r="B37" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1981,110 +2379,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
       <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.42578125" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="16.26953125" customWidth="1"/>
-    <col min="5" max="6" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.54296875" customWidth="1"/>
-    <col min="8" max="8" width="18.6328125" customWidth="1"/>
-    <col min="9" max="9" width="8.6328125" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.36328125" customWidth="1"/>
-    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" customWidth="1"/>
-    <col min="18" max="18" width="7.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="65.54296875" customWidth="1"/>
-    <col min="22" max="22" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="6" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.42578125" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" customWidth="1"/>
+    <col min="18" max="18" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="65.5703125" customWidth="1"/>
+    <col min="22" max="22" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="5.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="16"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="16"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="30"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="17"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="17"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="17"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>69</v>
       </c>
-      <c r="B8" s="17"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="17"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>71</v>
-      </c>
       <c r="B10" s="17"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B11" s="17"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="17"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2106,7 +2504,7 @@
       <c r="M15" s="26"/>
       <c r="N15" s="27"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>2</v>
       </c>
@@ -2117,36 +2515,36 @@
         <v>3</v>
       </c>
       <c r="D16" s="36" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="H16" s="36" t="s">
+        <v>67</v>
+      </c>
+      <c r="I16" s="36" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="K16" s="36" t="s">
         <v>72</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="F16" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="G16" s="36" t="s">
-        <v>67</v>
-      </c>
-      <c r="H16" s="36" t="s">
-        <v>68</v>
-      </c>
-      <c r="I16" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="K16" s="36" t="s">
-        <v>73</v>
       </c>
       <c r="L16" s="37" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -2182,7 +2580,7 @@
       <c r="L17" s="33"/>
       <c r="M17" s="18"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
         <v>7</v>
       </c>
@@ -2220,7 +2618,7 @@
       <c r="L18" s="33"/>
       <c r="M18" s="18"/>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="32" t="s">
         <v>8</v>
       </c>
@@ -2258,7 +2656,7 @@
       <c r="L19" s="34"/>
       <c r="M19" s="18"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="38" t="s">
         <v>2</v>
       </c>
@@ -2269,28 +2667,28 @@
         <v>3</v>
       </c>
       <c r="D20" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="I20" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="28" t="s">
         <v>72</v>
-      </c>
-      <c r="E20" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="I20" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="28" t="s">
-        <v>73</v>
       </c>
       <c r="L20" s="39" t="s">
         <v>5</v>

</xml_diff>